<commit_message>
Cambios para Formularios de CU agregados
</commit_message>
<xml_diff>
--- a/Formulario CU.xlsx
+++ b/Formulario CU.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jdgam\OneDrive\Documentos\Especialización\Diseño detallado de software\DDS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4637AEFF-398C-4313-A163-2DB73436D652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BD3C966-19E1-454D-B0AD-89115B35E854}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{CDB2E81D-813B-4043-98E1-42AECD8FB8FF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{CDB2E81D-813B-4043-98E1-42AECD8FB8FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="86">
   <si>
     <t xml:space="preserve">Código del caso De uso y nombre </t>
   </si>
@@ -69,9 +69,6 @@
   </si>
   <si>
     <t xml:space="preserve">Requisitos no Funcionales </t>
-  </si>
-  <si>
-    <t>CU-2021-01 Agregar articulos al carrito de compras</t>
   </si>
   <si>
     <t>El sistema debe permitir adicionar nuevos articulos al carrito de compras y debe actualizar la cantidad de articulos agregados, junto con el valor de la compra total</t>
@@ -156,9 +153,6 @@
     <t>Caso de Uso 1</t>
   </si>
   <si>
-    <t>CU-2021-02 Gestionar reclamos</t>
-  </si>
-  <si>
     <t>Cliente</t>
   </si>
   <si>
@@ -209,13 +203,108 @@
   </si>
   <si>
     <t>3 El sistema no encuentra elementos comprados</t>
+  </si>
+  <si>
+    <t>Caso de uso 3</t>
+  </si>
+  <si>
+    <t>Caso 3</t>
+  </si>
+  <si>
+    <t>CU004A Agregar articulos al carrito de compras</t>
+  </si>
+  <si>
+    <t>CU008 Administrar reclamos</t>
+  </si>
+  <si>
+    <t>CU007B Crear reclamos</t>
+  </si>
+  <si>
+    <t>CU003 Buscar productos</t>
+  </si>
+  <si>
+    <t>El sistema debe permitir a los asistentes administrar y modificar el estado de la reclamación</t>
+  </si>
+  <si>
+    <t>Bajo</t>
+  </si>
+  <si>
+    <t>Empleado</t>
+  </si>
+  <si>
+    <t>El empleado debe estar logeado
+El empleado debe usar la funcionalidad "Gestionar" para abrir el gestor y dar respuesta a un usuario final</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Opcion de Gestionar cuando se listan las reclamaciones, si se desea dar respuesta a una reclamación </t>
+  </si>
+  <si>
+    <t>El reclamo queda cerrado en el historico del producto</t>
+  </si>
+  <si>
+    <t>1 El administrador busca reclamaciones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 El administrador selecciona una reclamación de la lista </t>
+  </si>
+  <si>
+    <t>5 El administrador usa la funcionalidad Gestionar</t>
+  </si>
+  <si>
+    <t>2 El sistema despliega una lista con reclamaciones presentes</t>
+  </si>
+  <si>
+    <t>3 El sistema permite mostrar una lista filtrada con las reclamaciones encontradas</t>
+  </si>
+  <si>
+    <t>6 El sistema despliega una ventana que permite dar respuesta a la reclamación</t>
+  </si>
+  <si>
+    <t>7 El sistema actualiza el estado de la reclamación despues de ser revisada</t>
+  </si>
+  <si>
+    <t>3 El sistema no encuentra reclamaciones abiertas</t>
+  </si>
+  <si>
+    <t>El sistema debe permitir a clientes realizar busqueda por tipo de productos</t>
+  </si>
+  <si>
+    <t>El cliente debe estar logeado
+El cliente debe usar la funcionalidad "Buscar partes"</t>
+  </si>
+  <si>
+    <t>7 El sistema  no encuentra reclamaciones abiertas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Caso de uso 4 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Opcion de buscar partes para listar productos con tipo de marca e identificación </t>
+  </si>
+  <si>
+    <t>3 El sistema no encuentra elementos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Caso 4 </t>
+  </si>
+  <si>
+    <t>4 El cliente escribe el codigo del repuesto en la barra buscar</t>
+  </si>
+  <si>
+    <t>5 el sistema filtra la lista con los elementos encontrados</t>
+  </si>
+  <si>
+    <t>3 El sistema busca por categoria</t>
+  </si>
+  <si>
+    <t>5 El sistema  busca por código</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -248,6 +337,12 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -320,7 +415,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -334,24 +429,30 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -400,7 +501,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="Hoja2!$D$6:$E$10" spid="_x0000_s1075"/>
+                  <a14:cameraTool cellRange="Hoja2!$D$6:$E$10" spid="_x0000_s1107"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -440,15 +541,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>33616</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>46247</xdr:rowOff>
+      <xdr:colOff>22411</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>57452</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>7966885</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>1098177</xdr:rowOff>
+      <xdr:colOff>7955680</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>1109382</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -471,8 +572,96 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5244351" y="8024835"/>
+          <a:off x="5233146" y="12664070"/>
           <a:ext cx="7933269" cy="1051930"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>67236</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>67235</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>7956177</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>1098176</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Imagen 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3DD7E85B-79E3-4E40-AA18-F0D0B67F0C17}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5277971" y="8045823"/>
+          <a:ext cx="7888941" cy="1030941"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>78442</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>179294</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>7922560</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>884242</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Imagen 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{22B6EFCA-6E0B-4210-A54F-A943C998DBAC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5289177" y="17649265"/>
+          <a:ext cx="7844118" cy="704948"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -781,10 +970,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F469AC6F-0349-394E-A0A3-C9F55ABF679B}">
-  <dimension ref="C2:D32"/>
+  <dimension ref="C2:D63"/>
   <sheetViews>
-    <sheetView topLeftCell="B19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="B52" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D65" sqref="D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -794,23 +983,23 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C2" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="D2" s="11"/>
+      <c r="C2" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="13"/>
     </row>
     <row r="4" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C4" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="D4" s="14"/>
+      <c r="C4" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="15"/>
     </row>
     <row r="6" spans="3:4" ht="20.25" x14ac:dyDescent="0.3">
       <c r="C6" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>11</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="3:4" ht="32.25" x14ac:dyDescent="0.3">
@@ -818,7 +1007,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="3:4" ht="20.25" x14ac:dyDescent="0.3">
@@ -826,7 +1015,7 @@
         <v>2</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="3:4" ht="20.25" x14ac:dyDescent="0.3">
@@ -834,7 +1023,7 @@
         <v>3</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="3:4" ht="20.25" x14ac:dyDescent="0.3">
@@ -842,7 +1031,7 @@
         <v>4</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="3:4" ht="32.25" x14ac:dyDescent="0.3">
@@ -850,7 +1039,7 @@
         <v>5</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="3:4" ht="20.25" x14ac:dyDescent="0.3">
@@ -858,35 +1047,35 @@
         <v>6</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="3:4" ht="104.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="9"/>
+      <c r="D13" s="7"/>
     </row>
     <row r="14" spans="3:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D14" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C15" s="12"/>
+      <c r="D15" s="2" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C15" s="8"/>
-      <c r="D15" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="16" spans="3:4" ht="20.25" x14ac:dyDescent="0.3">
       <c r="C16" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="10" t="s">
-        <v>27</v>
+      <c r="D16" s="8" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="3:4" ht="20.25" x14ac:dyDescent="0.3">
@@ -896,21 +1085,21 @@
       <c r="D17" s="2"/>
     </row>
     <row r="18" spans="3:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="12"/>
-      <c r="D18" s="13"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="10"/>
     </row>
     <row r="19" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C19" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="D19" s="14"/>
+      <c r="C19" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="15"/>
     </row>
     <row r="21" spans="3:4" ht="20.25" x14ac:dyDescent="0.3">
       <c r="C21" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="3:4" ht="20.25" x14ac:dyDescent="0.3">
@@ -918,7 +1107,7 @@
         <v>1</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" spans="3:4" ht="20.25" x14ac:dyDescent="0.3">
@@ -926,7 +1115,7 @@
         <v>2</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>40</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="3:4" ht="20.25" x14ac:dyDescent="0.3">
@@ -934,7 +1123,7 @@
         <v>3</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="3:4" ht="20.25" x14ac:dyDescent="0.3">
@@ -942,7 +1131,7 @@
         <v>4</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>14</v>
+        <v>62</v>
       </c>
     </row>
     <row r="26" spans="3:4" ht="32.25" x14ac:dyDescent="0.3">
@@ -950,7 +1139,7 @@
         <v>5</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
     </row>
     <row r="27" spans="3:4" ht="20.25" x14ac:dyDescent="0.3">
@@ -958,35 +1147,33 @@
         <v>6</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
     </row>
     <row r="28" spans="3:4" ht="90" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C28" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D28" s="9"/>
+      <c r="D28" s="7"/>
     </row>
     <row r="29" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C29" s="7" t="s">
+      <c r="C29" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D29" s="2" t="s">
-        <v>56</v>
+      <c r="D29" s="16" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="30" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C30" s="8"/>
-      <c r="D30" s="2" t="s">
-        <v>55</v>
-      </c>
+      <c r="C30" s="12"/>
+      <c r="D30" s="17"/>
     </row>
     <row r="31" spans="3:4" ht="20.25" x14ac:dyDescent="0.3">
       <c r="C31" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D31" s="10" t="s">
-        <v>54</v>
+      <c r="D31" s="8" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="32" spans="3:4" ht="20.25" x14ac:dyDescent="0.3">
@@ -995,14 +1182,212 @@
       </c>
       <c r="D32" s="2"/>
     </row>
+    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C34" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="D34" s="15"/>
+    </row>
+    <row r="36" spans="3:4" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="C36" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="37" spans="3:4" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="C37" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="3:4" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="C38" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" spans="3:4" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="C39" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40" spans="3:4" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="C40" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="41" spans="3:4" ht="32.25" x14ac:dyDescent="0.3">
+      <c r="C41" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="3:4" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="C42" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="43" spans="3:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C43" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D43" s="7"/>
+    </row>
+    <row r="44" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C44" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="45" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C45" s="12"/>
+      <c r="D45" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="46" spans="3:4" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="C46" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="47" spans="3:4" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="C47" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D47" s="2"/>
+    </row>
+    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C50" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="D50" s="15"/>
+    </row>
+    <row r="52" spans="3:4" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="C52" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="53" spans="3:4" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="C53" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="54" spans="3:4" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="C54" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="55" spans="3:4" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="C55" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="56" spans="3:4" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="C56" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="57" spans="3:4" ht="32.25" x14ac:dyDescent="0.3">
+      <c r="C57" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="58" spans="3:4" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="C58" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="59" spans="3:4" ht="85.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C59" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D59" s="7"/>
+    </row>
+    <row r="60" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C60" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="61" spans="3:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C61" s="12"/>
+      <c r="D61" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="62" spans="3:4" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C62" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="63" spans="3:4" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="C63" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D63" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="10">
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="C60:C61"/>
+    <mergeCell ref="D29:D30"/>
     <mergeCell ref="C14:C15"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C29:C30"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="C4:D4"/>
   </mergeCells>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -1012,142 +1397,249 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DA116CA-1FE4-364A-ACA9-A85DBFFA4D9F}">
-  <dimension ref="D3:E27"/>
+  <dimension ref="D3:E53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E56" sqref="E56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="42.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.625" customWidth="1"/>
     <col min="5" max="5" width="77.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D3" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="E3" s="15"/>
+      <c r="D3" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" s="14"/>
     </row>
     <row r="5" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D5" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" t="s">
         <v>20</v>
-      </c>
-      <c r="E9" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="10" spans="4:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="E10" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D16" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="E16" s="14"/>
+      <c r="D16" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" s="15"/>
     </row>
     <row r="18" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D18" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="E19" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E20" t="s">
-        <v>50</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D22" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
       <c r="E22" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="23" spans="4:5" ht="31.5" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E23" s="4" t="s">
-        <v>52</v>
+        <v>73</v>
       </c>
     </row>
     <row r="25" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E26" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="29" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D29" s="14" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="27" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="E27" t="s">
-        <v>55</v>
+      <c r="E29" s="15"/>
+    </row>
+    <row r="31" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D31" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="32" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>45</v>
+      </c>
+      <c r="E32" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="33" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E33" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="34" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>46</v>
+      </c>
+      <c r="E35" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="36" spans="4:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E36" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="38" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="39" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E39" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="40" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E40" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="44" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D44" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E44" s="15"/>
+    </row>
+    <row r="46" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D46" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="47" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D47" t="s">
+        <v>16</v>
+      </c>
+      <c r="E47" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="48" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E48" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="49" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D49" t="s">
+        <v>82</v>
+      </c>
+      <c r="E49" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="51" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D51" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="52" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E52" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="53" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E53" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D44:E44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1165,34 +1657,34 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
         <v>30</v>
-      </c>
-      <c r="B2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
         <v>32</v>
-      </c>
-      <c r="B3" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" t="s">
         <v>34</v>
-      </c>
-      <c r="B4" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se crea diagrama de comunicacion
</commit_message>
<xml_diff>
--- a/Formulario CU.xlsx
+++ b/Formulario CU.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jdgam\OneDrive\Documentos\Especialización\Diseño detallado de software\DDS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nelsonpinzon/Library/Mobile Documents/com~apple~CloudDocs/Documents/Especialización/Diseño detallado de software/DDS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BD3C966-19E1-454D-B0AD-89115B35E854}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{444C4F7E-25FA-A74B-A4E5-955F20AA32C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{CDB2E81D-813B-4043-98E1-42AECD8FB8FF}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="1" xr2:uid="{CDB2E81D-813B-4043-98E1-42AECD8FB8FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="88">
   <si>
     <t xml:space="preserve">Código del caso De uso y nombre </t>
   </si>
@@ -96,9 +96,6 @@
     <t xml:space="preserve">4 El cliente selecciona un elemento de la lista </t>
   </si>
   <si>
-    <t>5 El cliente usa la funcionalidad agregar al carrito</t>
-  </si>
-  <si>
     <t>6 El sistema valida que el repuesto exista en el inventario</t>
   </si>
   <si>
@@ -298,6 +295,15 @@
   </si>
   <si>
     <t>5 El sistema  busca por código</t>
+  </si>
+  <si>
+    <t>1 el actor se encuentra con la lista filtrada de productos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 El actor selecciona un elemento de la lista </t>
+  </si>
+  <si>
+    <t>5 El actor usa la funcionalidad agregar al carrito</t>
   </si>
 </sst>
 </file>
@@ -433,19 +439,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -453,6 +456,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -501,7 +507,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="Hoja2!$D$6:$E$10" spid="_x0000_s1107"/>
+                  <a14:cameraTool cellRange="Hoja2!$D$6:$E$9" spid="_x0000_s1117"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -972,37 +978,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F469AC6F-0349-394E-A0A3-C9F55ABF679B}">
   <dimension ref="C2:D63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B52" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D65" sqref="D65"/>
+    <sheetView topLeftCell="B1" zoomScale="124" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="46.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="104.875" customWidth="1"/>
+    <col min="3" max="3" width="46.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="104.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C2" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" s="13"/>
-    </row>
-    <row r="4" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C4" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="D4" s="15"/>
-    </row>
-    <row r="6" spans="3:4" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="2" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C2" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="17"/>
+    </row>
+    <row r="4" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C4" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="12"/>
+    </row>
+    <row r="6" spans="3:4" ht="20" x14ac:dyDescent="0.2">
       <c r="C6" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="7" spans="3:4" ht="32.25" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="3:4" ht="34" x14ac:dyDescent="0.2">
       <c r="C7" s="1" t="s">
         <v>1</v>
       </c>
@@ -1010,15 +1016,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="3:4" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:4" ht="20" x14ac:dyDescent="0.2">
       <c r="C8" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="3:4" ht="20.25" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="3:4" ht="20" x14ac:dyDescent="0.2">
       <c r="C9" s="1" t="s">
         <v>3</v>
       </c>
@@ -1026,7 +1032,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="3:4" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:4" ht="20" x14ac:dyDescent="0.2">
       <c r="C10" s="1" t="s">
         <v>4</v>
       </c>
@@ -1034,7 +1040,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="3:4" ht="32.25" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:4" ht="34" x14ac:dyDescent="0.2">
       <c r="C11" s="1" t="s">
         <v>5</v>
       </c>
@@ -1042,7 +1048,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="3:4" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:4" ht="20" x14ac:dyDescent="0.2">
       <c r="C12" s="1" t="s">
         <v>6</v>
       </c>
@@ -1050,75 +1056,75 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="3:4" ht="104.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:4" ht="104" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C13" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="3:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="11" t="s">
+    <row r="14" spans="3:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C14" s="13" t="s">
         <v>8</v>
       </c>
       <c r="D14" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C15" s="14"/>
+      <c r="D15" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C15" s="12"/>
-      <c r="D15" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="3:4" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:4" ht="20" x14ac:dyDescent="0.2">
       <c r="C16" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="3:4" ht="20.25" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" ht="20" x14ac:dyDescent="0.2">
       <c r="C17" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="3:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C18" s="9"/>
       <c r="D18" s="10"/>
     </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C19" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="D19" s="15"/>
-    </row>
-    <row r="21" spans="3:4" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C19" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" s="12"/>
+    </row>
+    <row r="21" spans="3:4" ht="20" x14ac:dyDescent="0.2">
       <c r="C21" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="22" spans="3:4" ht="20.25" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="3:4" ht="20" x14ac:dyDescent="0.2">
       <c r="C22" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="23" spans="3:4" ht="20.25" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="3:4" ht="20" x14ac:dyDescent="0.2">
       <c r="C23" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="24" spans="3:4" ht="20.25" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="3:4" ht="20" x14ac:dyDescent="0.2">
       <c r="C24" s="1" t="s">
         <v>3</v>
       </c>
@@ -1126,93 +1132,93 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="3:4" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:4" ht="20" x14ac:dyDescent="0.2">
       <c r="C25" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="26" spans="3:4" ht="32.25" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" spans="3:4" ht="34" x14ac:dyDescent="0.2">
       <c r="C26" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="27" spans="3:4" ht="20.25" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="27" spans="3:4" ht="20" x14ac:dyDescent="0.2">
       <c r="C27" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="28" spans="3:4" ht="90" customHeight="1" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="3:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C28" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D28" s="7"/>
     </row>
-    <row r="29" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C29" s="11" t="s">
+    <row r="29" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C29" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D29" s="16" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="30" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C30" s="12"/>
-      <c r="D30" s="17"/>
-    </row>
-    <row r="31" spans="3:4" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="D29" s="15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="30" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C30" s="14"/>
+      <c r="D30" s="16"/>
+    </row>
+    <row r="31" spans="3:4" ht="20" x14ac:dyDescent="0.2">
       <c r="C31" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="32" spans="3:4" ht="20.25" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="32" spans="3:4" ht="20" x14ac:dyDescent="0.2">
       <c r="C32" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D32" s="2"/>
     </row>
-    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C34" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="D34" s="15"/>
-    </row>
-    <row r="36" spans="3:4" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C34" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D34" s="12"/>
+    </row>
+    <row r="36" spans="3:4" ht="20" x14ac:dyDescent="0.2">
       <c r="C36" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="37" spans="3:4" ht="20.25" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="37" spans="3:4" ht="20" x14ac:dyDescent="0.2">
       <c r="C37" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="38" spans="3:4" ht="20.25" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="38" spans="3:4" ht="20" x14ac:dyDescent="0.2">
       <c r="C38" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="39" spans="3:4" ht="20.25" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="3:4" ht="20" x14ac:dyDescent="0.2">
       <c r="C39" s="1" t="s">
         <v>3</v>
       </c>
@@ -1220,7 +1226,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="40" spans="3:4" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:4" ht="20" x14ac:dyDescent="0.2">
       <c r="C40" s="1" t="s">
         <v>4</v>
       </c>
@@ -1228,87 +1234,87 @@
         <v>13</v>
       </c>
     </row>
-    <row r="41" spans="3:4" ht="32.25" x14ac:dyDescent="0.3">
+    <row r="41" spans="3:4" ht="34" x14ac:dyDescent="0.2">
       <c r="C41" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="42" spans="3:4" ht="20.25" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="3:4" ht="20" x14ac:dyDescent="0.2">
       <c r="C42" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="43" spans="3:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="43" spans="3:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C43" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D43" s="7"/>
     </row>
-    <row r="44" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C44" s="11" t="s">
+    <row r="44" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C44" s="13" t="s">
         <v>8</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="45" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C45" s="12"/>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="45" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C45" s="14"/>
       <c r="D45" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="46" spans="3:4" ht="20.25" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="46" spans="3:4" ht="20" x14ac:dyDescent="0.2">
       <c r="C46" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="47" spans="3:4" ht="20.25" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="47" spans="3:4" ht="20" x14ac:dyDescent="0.2">
       <c r="C47" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D47" s="2"/>
     </row>
-    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C50" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="D50" s="15"/>
-    </row>
-    <row r="52" spans="3:4" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="50" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C50" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="D50" s="12"/>
+    </row>
+    <row r="52" spans="3:4" ht="20" x14ac:dyDescent="0.2">
       <c r="C52" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="53" spans="3:4" ht="20.25" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="53" spans="3:4" ht="20" x14ac:dyDescent="0.2">
       <c r="C53" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="54" spans="3:4" ht="20.25" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="54" spans="3:4" ht="20" x14ac:dyDescent="0.2">
       <c r="C54" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="55" spans="3:4" ht="20.25" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="55" spans="3:4" ht="20" x14ac:dyDescent="0.2">
       <c r="C55" s="1" t="s">
         <v>3</v>
       </c>
@@ -1316,59 +1322,59 @@
         <v>13</v>
       </c>
     </row>
-    <row r="56" spans="3:4" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="56" spans="3:4" ht="20" x14ac:dyDescent="0.2">
       <c r="C56" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="57" spans="3:4" ht="32.25" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="57" spans="3:4" ht="34" x14ac:dyDescent="0.2">
       <c r="C57" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="58" spans="3:4" ht="20.25" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="58" spans="3:4" ht="20" x14ac:dyDescent="0.2">
       <c r="C58" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="59" spans="3:4" ht="85.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="59" spans="3:4" ht="85.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C59" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D59" s="7"/>
     </row>
-    <row r="60" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C60" s="11" t="s">
+    <row r="60" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C60" s="13" t="s">
         <v>8</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="61" spans="3:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C61" s="12"/>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="61" spans="3:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C61" s="14"/>
       <c r="D61" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="62" spans="3:4" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="62" spans="3:4" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C62" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="63" spans="3:4" ht="20.25" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="63" spans="3:4" ht="20" x14ac:dyDescent="0.2">
       <c r="C63" s="1" t="s">
         <v>10</v>
       </c>
@@ -1376,16 +1382,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C4:D4"/>
     <mergeCell ref="C34:D34"/>
     <mergeCell ref="C44:C45"/>
     <mergeCell ref="C50:D50"/>
     <mergeCell ref="C60:C61"/>
     <mergeCell ref="D29:D30"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C4:D4"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1399,239 +1405,231 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DA116CA-1FE4-364A-ACA9-A85DBFFA4D9F}">
   <dimension ref="D3:E53"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E56" sqref="E56"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="51.625" customWidth="1"/>
-    <col min="5" max="5" width="77.375" customWidth="1"/>
+    <col min="4" max="4" width="51.6640625" customWidth="1"/>
+    <col min="5" max="5" width="77.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D3" s="14" t="s">
+    <row r="3" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D3" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="11"/>
+    </row>
+    <row r="5" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D5" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D8" t="s">
+        <v>87</v>
+      </c>
+      <c r="E8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="4:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="E9" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="E13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="E14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D16" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="E3" s="14"/>
-    </row>
-    <row r="5" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D5" s="5" t="s">
+      <c r="E16" s="12"/>
+    </row>
+    <row r="18" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D18" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="5" t="s">
+    </row>
+    <row r="19" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D19" t="s">
+        <v>66</v>
+      </c>
+      <c r="E19" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="E20" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D21" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D22" t="s">
+        <v>68</v>
+      </c>
+      <c r="E22" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="4:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E23" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D25" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="E26" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D29" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="E29" s="12"/>
+    </row>
+    <row r="31" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D31" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="32" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D32" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="6" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="E7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="4:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="E10" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="E13" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="E14" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D16" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="E16" s="15"/>
-    </row>
-    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D18" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D19" t="s">
-        <v>67</v>
-      </c>
-      <c r="E19" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="20" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="E20" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="21" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D21" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="22" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D22" t="s">
-        <v>69</v>
-      </c>
-      <c r="E22" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="23" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="E23" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="25" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D25" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="26" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="E26" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="29" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D29" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="E29" s="15"/>
-    </row>
-    <row r="31" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D31" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="32" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D32" t="s">
-        <v>45</v>
-      </c>
       <c r="E32" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="E33" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="33" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="E33" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="34" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D34" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D35" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E35" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="36" spans="4:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="E36" s="4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="36" spans="4:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="E36" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="38" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D38" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="39" spans="4:5" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="4:5" x14ac:dyDescent="0.2">
       <c r="E39" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="40" spans="4:5" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="40" spans="4:5" x14ac:dyDescent="0.2">
       <c r="E40" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="44" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D44" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E44" s="15"/>
-    </row>
-    <row r="46" spans="4:5" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="44" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D44" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="E44" s="12"/>
+    </row>
+    <row r="46" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D46" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E46" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="E46" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="47" spans="4:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D47" t="s">
         <v>16</v>
       </c>
       <c r="E47" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="48" spans="4:5" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="48" spans="4:5" x14ac:dyDescent="0.2">
       <c r="E48" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="49" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D49" t="s">
+        <v>81</v>
+      </c>
+      <c r="E49" t="s">
         <v>82</v>
       </c>
-      <c r="E49" t="s">
+    </row>
+    <row r="51" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D51" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="52" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="E52" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="51" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D51" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="52" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="E52" t="s">
+    <row r="53" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="E53" t="s">
         <v>84</v>
-      </c>
-    </row>
-    <row r="53" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="E53" t="s">
-        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1653,38 +1651,38 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>28</v>
       </c>
-      <c r="B1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>29</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
         <v>31</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="B4" t="s">
         <v>33</v>
-      </c>
-      <c r="B4" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>